<commit_message>
Revert "add new Rachel neut data set 2 & configure `yaml`"
This reverts commit 648f9e8b3ace0bc742ee603fcb86b171235081e9.
</commit_message>
<xml_diff>
--- a/data/neut_assays/plate_reader_data/fPitt3postinf_NeutralizationAssay.xlsx
+++ b/data/neut_assays/plate_reader_data/fPitt3postinf_NeutralizationAssay.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" activeTab="6"/>
+    <workbookView xWindow="34120" yWindow="460" windowWidth="28800" windowHeight="16400" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="WT" sheetId="2" r:id="rId1"/>
@@ -17,8 +17,6 @@
     <sheet name="F193D" sheetId="3" r:id="rId3"/>
     <sheet name="K160T" sheetId="4" r:id="rId4"/>
     <sheet name="L157D" sheetId="5" r:id="rId5"/>
-    <sheet name="WT2" sheetId="6" r:id="rId6"/>
-    <sheet name="R220D" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -477,186 +475,8 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Eguia, Rachel T</author>
-  </authors>
-  <commentList>
-    <comment ref="E1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Tecan.At.Common, 3.3.10.0
-Tecan.At.Common.DocumentManagement, 3.3.10.0
-Tecan.At.Common.DocumentManagement.Reader, 3.1.17.0
-Tecan.At.Common.MCS, 3.3.10.0
-Tecan.At.Common.Results, 3.3.10.0
-Tecan.At.Common.UI, 3.3.10.0
-Tecan.At.Communication.Common, 3.3.12.0
-Tecan.At.Communication.Port.IP, 3.3.12.0
-Tecan.At.Communication.Port.RS232, 3.3.12.0
-Tecan.At.Communication.Port.SIM.Common, 3.3.12.0
-Tecan.At.Communication.Port.USB, 3.3.12.0
-Tecan.At.Communication.Server, 3.3.12.0
-Tecan.At.Communication.SIM.AMR, 3.1.17.0
-Tecan.At.Communication.SIM.AMRPlus, 3.1.17.0
-Tecan.At.Communication.SIM.Connect, 3.3.12.0
-Tecan.At.Communication.SIM.GeniosUltra, 3.1.17.0
-Tecan.At.Communication.SIM.Safire3, 3.1.17.0
-Tecan.At.Communication.SIM.Safire3Pro, 3.1.17.0
-Tecan.At.Communication.SIM.SunriseMini, 3.1.17.0
-Tecan.At.Instrument.Common, 3.3.12.0
-Tecan.At.Instrument.Common.Reader, 3.1.17.0
-Tecan.At.Instrument.Common.Stacker, 3.3.12.0
-Tecan.At.Instrument.Reader.AMR, 3.1.17.0
-Tecan.At.Instrument.Reader.AMRPlus, 3.1.17.0
-Tecan.At.Instrument.Reader.GeniosUltra, 3.1.17.0
-Tecan.At.Instrument.Reader.Safire3, 3.1.17.0
-Tecan.At.Instrument.Reader.Safire3Pro, 3.1.17.0
-Tecan.At.Instrument.Reader.SunriseMini, 3.1.17.0
-Tecan.At.Instrument.Server, 3.3.12.0
-Tecan.At.Instrument.Stacker.Connect, 3.3.12.0
-Tecan.At.Instrument.Stacker.Server, 3.3.12.0
-Tecan.At.Measurement.BuiltInTest.Common, 3.1.17.0
-Tecan.At.Measurement.Common, 3.1.17.0
-Tecan.At.Measurement.Server, 3.1.17.0
-Tecan.At.XFluor, 1.9.17.0
-Tecan.At.XFluor.Connect.Reader, 1.9.17.0
-Tecan.At.XFluor.Core, 1.9.17.0
-Tecan.At.XFluor.Device, 1.9.17.0
-Tecan.At.XFluor.Device.AMR, 1.9.17.0
-Tecan.At.XFluor.Device.AMRPlus, 1.9.17.0
-Tecan.At.XFluor.Device.GeniosUltra, 1.9.17.0
-Tecan.At.XFluor.Device.Reader, 1.9.17.0
-Tecan.At.XFluor.Device.Safire3, 1.9.17.0
-Tecan.At.XFluor.Device.Safire3Pro, 1.9.17.0
-Tecan.At.XFluor.Device.SunriseMini, 1.9.17.0
-Tecan.At.XFluor.ExcelOutput, 1.9.17.0
-Tecan.At.XFluor.NanoQuant, 1.9.17.0
-Tecan.At.XFluor.ReaderEditor, 1.9.17.0
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
-MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
-ABS, V 1.00 MCR Abs 4 Channel (V 1.00 MCR Abs 4 Channel)
-LUM, V_1.04_11/2011_LUMINESCENCE (Nov 02 2011/17.53.34)
-TCAN, V_1.00_02/2008_S3FTCAN (Feb 21 2008/17.19.16)
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Eguia, Rachel T</author>
-  </authors>
-  <commentList>
-    <comment ref="E1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Tecan.At.Common, 3.3.10.0
-Tecan.At.Common.DocumentManagement, 3.3.10.0
-Tecan.At.Common.DocumentManagement.Reader, 3.1.17.0
-Tecan.At.Common.MCS, 3.3.10.0
-Tecan.At.Common.Results, 3.3.10.0
-Tecan.At.Common.UI, 3.3.10.0
-Tecan.At.Communication.Common, 3.3.12.0
-Tecan.At.Communication.Port.IP, 3.3.12.0
-Tecan.At.Communication.Port.RS232, 3.3.12.0
-Tecan.At.Communication.Port.SIM.Common, 3.3.12.0
-Tecan.At.Communication.Port.USB, 3.3.12.0
-Tecan.At.Communication.Server, 3.3.12.0
-Tecan.At.Communication.SIM.AMR, 3.1.17.0
-Tecan.At.Communication.SIM.AMRPlus, 3.1.17.0
-Tecan.At.Communication.SIM.Connect, 3.3.12.0
-Tecan.At.Communication.SIM.GeniosUltra, 3.1.17.0
-Tecan.At.Communication.SIM.Safire3, 3.1.17.0
-Tecan.At.Communication.SIM.Safire3Pro, 3.1.17.0
-Tecan.At.Communication.SIM.SunriseMini, 3.1.17.0
-Tecan.At.Instrument.Common, 3.3.12.0
-Tecan.At.Instrument.Common.Reader, 3.1.17.0
-Tecan.At.Instrument.Common.Stacker, 3.3.12.0
-Tecan.At.Instrument.Reader.AMR, 3.1.17.0
-Tecan.At.Instrument.Reader.AMRPlus, 3.1.17.0
-Tecan.At.Instrument.Reader.GeniosUltra, 3.1.17.0
-Tecan.At.Instrument.Reader.Safire3, 3.1.17.0
-Tecan.At.Instrument.Reader.Safire3Pro, 3.1.17.0
-Tecan.At.Instrument.Reader.SunriseMini, 3.1.17.0
-Tecan.At.Instrument.Server, 3.3.12.0
-Tecan.At.Instrument.Stacker.Connect, 3.3.12.0
-Tecan.At.Instrument.Stacker.Server, 3.3.12.0
-Tecan.At.Measurement.BuiltInTest.Common, 3.1.17.0
-Tecan.At.Measurement.Common, 3.1.17.0
-Tecan.At.Measurement.Server, 3.1.17.0
-Tecan.At.XFluor, 1.9.17.0
-Tecan.At.XFluor.Connect.Reader, 1.9.17.0
-Tecan.At.XFluor.Core, 1.9.17.0
-Tecan.At.XFluor.Device, 1.9.17.0
-Tecan.At.XFluor.Device.AMR, 1.9.17.0
-Tecan.At.XFluor.Device.AMRPlus, 1.9.17.0
-Tecan.At.XFluor.Device.GeniosUltra, 1.9.17.0
-Tecan.At.XFluor.Device.Reader, 1.9.17.0
-Tecan.At.XFluor.Device.Safire3, 1.9.17.0
-Tecan.At.XFluor.Device.Safire3Pro, 1.9.17.0
-Tecan.At.XFluor.Device.SunriseMini, 1.9.17.0
-Tecan.At.XFluor.ExcelOutput, 1.9.17.0
-Tecan.At.XFluor.NanoQuant, 1.9.17.0
-Tecan.At.XFluor.ReaderEditor, 1.9.17.0
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
-MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
-ABS, V 1.00 MCR Abs 4 Channel (V 1.00 MCR Abs 4 Channel)
-LUM, V_1.04_11/2011_LUMINESCENCE (Nov 02 2011/17.53.34)
-TCAN, V_1.00_02/2008_S3FTCAN (Feb 21 2008/17.19.16)
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="64">
   <si>
     <t>Application: Tecan i-control</t>
   </si>
@@ -848,30 +668,6 @@
   </si>
   <si>
     <t>H</t>
-  </si>
-  <si>
-    <t>9:38:04 AM</t>
-  </si>
-  <si>
-    <t>FHCRC\reguia</t>
-  </si>
-  <si>
-    <t>5/24/2019 9:39:01 AM</t>
-  </si>
-  <si>
-    <t>5/24/2019 9:39:57 AM</t>
-  </si>
-  <si>
-    <t>9:35:52 AM</t>
-  </si>
-  <si>
-    <t>5/24/2019 9:36:49 AM</t>
-  </si>
-  <si>
-    <t>Temperature: 24.1 °C</t>
-  </si>
-  <si>
-    <t>5/24/2019 9:37:45 AM</t>
   </si>
 </sst>
 </file>
@@ -3481,7 +3277,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A32" sqref="A32:A39"/>
     </sheetView>
   </sheetViews>
@@ -4007,1210 +3803,4 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M43"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
-        <v>43609</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18">
-        <v>485</v>
-      </c>
-      <c r="F18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19">
-        <v>515</v>
-      </c>
-      <c r="F19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20">
-        <v>12</v>
-      </c>
-      <c r="F20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21">
-        <v>12</v>
-      </c>
-      <c r="F21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22">
-        <v>107</v>
-      </c>
-      <c r="F22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E23">
-        <v>25</v>
-      </c>
-      <c r="F23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>29</v>
-      </c>
-      <c r="E24">
-        <v>400</v>
-      </c>
-      <c r="F24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>31</v>
-      </c>
-      <c r="E25">
-        <v>20</v>
-      </c>
-      <c r="F25" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>33</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>34</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B31" s="3">
-        <v>1</v>
-      </c>
-      <c r="C31" s="3">
-        <v>2</v>
-      </c>
-      <c r="D31" s="3">
-        <v>3</v>
-      </c>
-      <c r="E31" s="3">
-        <v>4</v>
-      </c>
-      <c r="F31" s="3">
-        <v>5</v>
-      </c>
-      <c r="G31" s="3">
-        <v>6</v>
-      </c>
-      <c r="H31" s="3">
-        <v>7</v>
-      </c>
-      <c r="I31" s="3">
-        <v>8</v>
-      </c>
-      <c r="J31" s="3">
-        <v>9</v>
-      </c>
-      <c r="K31" s="3">
-        <v>10</v>
-      </c>
-      <c r="L31" s="3">
-        <v>11</v>
-      </c>
-      <c r="M31" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32">
-        <v>12327</v>
-      </c>
-      <c r="C32">
-        <v>12760</v>
-      </c>
-      <c r="D32">
-        <v>12959</v>
-      </c>
-      <c r="E32">
-        <v>13124</v>
-      </c>
-      <c r="F32">
-        <v>13753</v>
-      </c>
-      <c r="G32">
-        <v>13678</v>
-      </c>
-      <c r="H32">
-        <v>13414</v>
-      </c>
-      <c r="I32">
-        <v>13220</v>
-      </c>
-      <c r="J32">
-        <v>13209</v>
-      </c>
-      <c r="K32">
-        <v>12995</v>
-      </c>
-      <c r="L32">
-        <v>12681</v>
-      </c>
-      <c r="M32">
-        <v>12051</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33">
-        <v>18369</v>
-      </c>
-      <c r="C33">
-        <v>18754</v>
-      </c>
-      <c r="D33">
-        <v>19148</v>
-      </c>
-      <c r="E33">
-        <v>18976</v>
-      </c>
-      <c r="F33">
-        <v>19302</v>
-      </c>
-      <c r="G33">
-        <v>19273</v>
-      </c>
-      <c r="H33">
-        <v>19058</v>
-      </c>
-      <c r="I33">
-        <v>19133</v>
-      </c>
-      <c r="J33">
-        <v>19066</v>
-      </c>
-      <c r="K33">
-        <v>18721</v>
-      </c>
-      <c r="L33">
-        <v>18657</v>
-      </c>
-      <c r="M33">
-        <v>18449</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B34">
-        <v>30983</v>
-      </c>
-      <c r="C34">
-        <v>33364</v>
-      </c>
-      <c r="D34">
-        <v>35331</v>
-      </c>
-      <c r="E34">
-        <v>37558</v>
-      </c>
-      <c r="F34">
-        <v>38574</v>
-      </c>
-      <c r="G34">
-        <v>38284</v>
-      </c>
-      <c r="H34">
-        <v>36053</v>
-      </c>
-      <c r="I34">
-        <v>36243</v>
-      </c>
-      <c r="J34">
-        <v>36523</v>
-      </c>
-      <c r="K34">
-        <v>37485</v>
-      </c>
-      <c r="L34">
-        <v>34632</v>
-      </c>
-      <c r="M34">
-        <v>34497</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B35">
-        <v>32556</v>
-      </c>
-      <c r="C35">
-        <v>32516</v>
-      </c>
-      <c r="D35">
-        <v>35038</v>
-      </c>
-      <c r="E35">
-        <v>34913</v>
-      </c>
-      <c r="F35">
-        <v>31444</v>
-      </c>
-      <c r="G35">
-        <v>29245</v>
-      </c>
-      <c r="H35">
-        <v>23503</v>
-      </c>
-      <c r="I35">
-        <v>19900</v>
-      </c>
-      <c r="J35">
-        <v>18850</v>
-      </c>
-      <c r="K35">
-        <v>20109</v>
-      </c>
-      <c r="L35">
-        <v>22352</v>
-      </c>
-      <c r="M35">
-        <v>28901</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B36">
-        <v>32535</v>
-      </c>
-      <c r="C36">
-        <v>34674</v>
-      </c>
-      <c r="D36">
-        <v>33007</v>
-      </c>
-      <c r="E36">
-        <v>34508</v>
-      </c>
-      <c r="F36">
-        <v>32526</v>
-      </c>
-      <c r="G36">
-        <v>29061</v>
-      </c>
-      <c r="H36">
-        <v>23703</v>
-      </c>
-      <c r="I36">
-        <v>19991</v>
-      </c>
-      <c r="J36">
-        <v>18777</v>
-      </c>
-      <c r="K36">
-        <v>19743</v>
-      </c>
-      <c r="L36">
-        <v>22617</v>
-      </c>
-      <c r="M36">
-        <v>28693</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B37">
-        <v>29808</v>
-      </c>
-      <c r="C37">
-        <v>32390</v>
-      </c>
-      <c r="D37">
-        <v>32201</v>
-      </c>
-      <c r="E37">
-        <v>30991</v>
-      </c>
-      <c r="F37">
-        <v>30605</v>
-      </c>
-      <c r="G37">
-        <v>26908</v>
-      </c>
-      <c r="H37">
-        <v>23552</v>
-      </c>
-      <c r="I37">
-        <v>20123</v>
-      </c>
-      <c r="J37">
-        <v>18665</v>
-      </c>
-      <c r="K37">
-        <v>19748</v>
-      </c>
-      <c r="L37">
-        <v>22626</v>
-      </c>
-      <c r="M37">
-        <v>28373</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38">
-        <v>29534</v>
-      </c>
-      <c r="C38">
-        <v>32376</v>
-      </c>
-      <c r="D38">
-        <v>33415</v>
-      </c>
-      <c r="E38">
-        <v>32909</v>
-      </c>
-      <c r="F38">
-        <v>33462</v>
-      </c>
-      <c r="G38">
-        <v>34611</v>
-      </c>
-      <c r="H38">
-        <v>33097</v>
-      </c>
-      <c r="I38">
-        <v>36800</v>
-      </c>
-      <c r="J38">
-        <v>34956</v>
-      </c>
-      <c r="K38">
-        <v>33615</v>
-      </c>
-      <c r="L38">
-        <v>32814</v>
-      </c>
-      <c r="M38">
-        <v>31940</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B39">
-        <v>11215</v>
-      </c>
-      <c r="C39">
-        <v>12188</v>
-      </c>
-      <c r="D39">
-        <v>11824</v>
-      </c>
-      <c r="E39">
-        <v>12283</v>
-      </c>
-      <c r="F39">
-        <v>12468</v>
-      </c>
-      <c r="G39">
-        <v>12499</v>
-      </c>
-      <c r="H39">
-        <v>12566</v>
-      </c>
-      <c r="I39">
-        <v>12364</v>
-      </c>
-      <c r="J39">
-        <v>12240</v>
-      </c>
-      <c r="K39">
-        <v>11947</v>
-      </c>
-      <c r="L39">
-        <v>11525</v>
-      </c>
-      <c r="M39">
-        <v>11224</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>46</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M43"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
-        <v>43609</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18">
-        <v>485</v>
-      </c>
-      <c r="F18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19">
-        <v>515</v>
-      </c>
-      <c r="F19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20">
-        <v>12</v>
-      </c>
-      <c r="F20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21">
-        <v>12</v>
-      </c>
-      <c r="F21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22">
-        <v>106</v>
-      </c>
-      <c r="F22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E23">
-        <v>25</v>
-      </c>
-      <c r="F23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>29</v>
-      </c>
-      <c r="E24">
-        <v>400</v>
-      </c>
-      <c r="F24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>31</v>
-      </c>
-      <c r="E25">
-        <v>20</v>
-      </c>
-      <c r="F25" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>33</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>34</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B31" s="3">
-        <v>1</v>
-      </c>
-      <c r="C31" s="3">
-        <v>2</v>
-      </c>
-      <c r="D31" s="3">
-        <v>3</v>
-      </c>
-      <c r="E31" s="3">
-        <v>4</v>
-      </c>
-      <c r="F31" s="3">
-        <v>5</v>
-      </c>
-      <c r="G31" s="3">
-        <v>6</v>
-      </c>
-      <c r="H31" s="3">
-        <v>7</v>
-      </c>
-      <c r="I31" s="3">
-        <v>8</v>
-      </c>
-      <c r="J31" s="3">
-        <v>9</v>
-      </c>
-      <c r="K31" s="3">
-        <v>10</v>
-      </c>
-      <c r="L31" s="3">
-        <v>11</v>
-      </c>
-      <c r="M31" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32">
-        <v>11365</v>
-      </c>
-      <c r="C32">
-        <v>11575</v>
-      </c>
-      <c r="D32">
-        <v>12419</v>
-      </c>
-      <c r="E32">
-        <v>12620</v>
-      </c>
-      <c r="F32">
-        <v>12784</v>
-      </c>
-      <c r="G32">
-        <v>12827</v>
-      </c>
-      <c r="H32">
-        <v>12794</v>
-      </c>
-      <c r="I32">
-        <v>12185</v>
-      </c>
-      <c r="J32">
-        <v>12777</v>
-      </c>
-      <c r="K32">
-        <v>11856</v>
-      </c>
-      <c r="L32">
-        <v>11664</v>
-      </c>
-      <c r="M32">
-        <v>11273</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33">
-        <v>16342</v>
-      </c>
-      <c r="C33">
-        <v>16507</v>
-      </c>
-      <c r="D33">
-        <v>16806</v>
-      </c>
-      <c r="E33">
-        <v>17198</v>
-      </c>
-      <c r="F33">
-        <v>17249</v>
-      </c>
-      <c r="G33">
-        <v>17491</v>
-      </c>
-      <c r="H33">
-        <v>17128</v>
-      </c>
-      <c r="I33">
-        <v>17333</v>
-      </c>
-      <c r="J33">
-        <v>17006</v>
-      </c>
-      <c r="K33">
-        <v>16956</v>
-      </c>
-      <c r="L33">
-        <v>16246</v>
-      </c>
-      <c r="M33">
-        <v>16266</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B34">
-        <v>29891</v>
-      </c>
-      <c r="C34">
-        <v>31200</v>
-      </c>
-      <c r="D34">
-        <v>30236</v>
-      </c>
-      <c r="E34">
-        <v>28736</v>
-      </c>
-      <c r="F34">
-        <v>30446</v>
-      </c>
-      <c r="G34">
-        <v>33313</v>
-      </c>
-      <c r="H34">
-        <v>35451</v>
-      </c>
-      <c r="I34">
-        <v>31579</v>
-      </c>
-      <c r="J34">
-        <v>32933</v>
-      </c>
-      <c r="K34">
-        <v>32589</v>
-      </c>
-      <c r="L34">
-        <v>33573</v>
-      </c>
-      <c r="M34">
-        <v>30806</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B35">
-        <v>27413</v>
-      </c>
-      <c r="C35">
-        <v>27513</v>
-      </c>
-      <c r="D35">
-        <v>26654</v>
-      </c>
-      <c r="E35">
-        <v>23405</v>
-      </c>
-      <c r="F35">
-        <v>19786</v>
-      </c>
-      <c r="G35">
-        <v>17247</v>
-      </c>
-      <c r="H35">
-        <v>16929</v>
-      </c>
-      <c r="I35">
-        <v>17012</v>
-      </c>
-      <c r="J35">
-        <v>17037</v>
-      </c>
-      <c r="K35">
-        <v>17900</v>
-      </c>
-      <c r="L35">
-        <v>20319</v>
-      </c>
-      <c r="M35">
-        <v>25495</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B36">
-        <v>29514</v>
-      </c>
-      <c r="C36">
-        <v>29011</v>
-      </c>
-      <c r="D36">
-        <v>27239</v>
-      </c>
-      <c r="E36">
-        <v>23082</v>
-      </c>
-      <c r="F36">
-        <v>19157</v>
-      </c>
-      <c r="G36">
-        <v>17155</v>
-      </c>
-      <c r="H36">
-        <v>16597</v>
-      </c>
-      <c r="I36">
-        <v>16404</v>
-      </c>
-      <c r="J36">
-        <v>16774</v>
-      </c>
-      <c r="K36">
-        <v>17663</v>
-      </c>
-      <c r="L36">
-        <v>20162</v>
-      </c>
-      <c r="M36">
-        <v>25509</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B37">
-        <v>28661</v>
-      </c>
-      <c r="C37">
-        <v>29045</v>
-      </c>
-      <c r="D37">
-        <v>25959</v>
-      </c>
-      <c r="E37">
-        <v>23264</v>
-      </c>
-      <c r="F37">
-        <v>18431</v>
-      </c>
-      <c r="G37">
-        <v>16842</v>
-      </c>
-      <c r="H37">
-        <v>16474</v>
-      </c>
-      <c r="I37">
-        <v>16342</v>
-      </c>
-      <c r="J37">
-        <v>16407</v>
-      </c>
-      <c r="K37">
-        <v>17526</v>
-      </c>
-      <c r="L37">
-        <v>19933</v>
-      </c>
-      <c r="M37">
-        <v>25128</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38">
-        <v>28160</v>
-      </c>
-      <c r="C38">
-        <v>29027</v>
-      </c>
-      <c r="D38">
-        <v>28325</v>
-      </c>
-      <c r="E38">
-        <v>29504</v>
-      </c>
-      <c r="F38">
-        <v>30528</v>
-      </c>
-      <c r="G38">
-        <v>29276</v>
-      </c>
-      <c r="H38">
-        <v>31266</v>
-      </c>
-      <c r="I38">
-        <v>30390</v>
-      </c>
-      <c r="J38">
-        <v>30010</v>
-      </c>
-      <c r="K38">
-        <v>30887</v>
-      </c>
-      <c r="L38">
-        <v>28374</v>
-      </c>
-      <c r="M38">
-        <v>29486</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B39">
-        <v>10798</v>
-      </c>
-      <c r="C39">
-        <v>10819</v>
-      </c>
-      <c r="D39">
-        <v>11096</v>
-      </c>
-      <c r="E39">
-        <v>11337</v>
-      </c>
-      <c r="F39">
-        <v>11569</v>
-      </c>
-      <c r="G39">
-        <v>11746</v>
-      </c>
-      <c r="H39">
-        <v>11609</v>
-      </c>
-      <c r="I39">
-        <v>11497</v>
-      </c>
-      <c r="J39">
-        <v>11382</v>
-      </c>
-      <c r="K39">
-        <v>11200</v>
-      </c>
-      <c r="L39">
-        <v>10498</v>
-      </c>
-      <c r="M39">
-        <v>10255</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>46</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>